<commit_message>
edited AVG_MAIN to not inherit TEST classes
</commit_message>
<xml_diff>
--- a/Report - Copy.xlsx
+++ b/Report - Copy.xlsx
@@ -4201,7 +4201,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>03/10-21:33</t>
+          <t>04/10-12:54</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -4211,7 +4211,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>03/10-21:35</t>
+          <t>04/10-12:55</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -4221,7 +4221,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>03/10-21:36</t>
+          <t>04/10-12:57</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -4231,7 +4231,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>03/10-21:38</t>
+          <t>04/10-12:58</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -4241,7 +4241,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>03/10-21:40</t>
+          <t>04/10-13:00</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -4251,7 +4251,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>03/10-21:42</t>
+          <t>04/10-13:01</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -4261,7 +4261,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>03/10-21:44</t>
+          <t>04/10-13:03</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -4271,17 +4271,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>03/10-21:47</t>
+          <t>04/10-13:04</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>95</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>03/10-21:50</t>
+          <t>04/10-13:06</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -4291,7 +4291,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>03/10-21:53</t>
+          <t>04/10-13:07</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -4301,7 +4301,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>03/10-21:55</t>
+          <t>04/10-13:08</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -4311,7 +4311,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>03/10-21:57</t>
+          <t>04/10-13:10</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -4321,7 +4321,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>03/10-22:00</t>
+          <t>04/10-13:11</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -4331,7 +4331,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>03/10-22:02</t>
+          <t>04/10-13:13</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -4341,7 +4341,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>03/10-22:04</t>
+          <t>04/10-13:14</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -4351,7 +4351,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>03/10-22:06</t>
+          <t>04/10-13:16</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -4361,7 +4361,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>03/10-22:08</t>
+          <t>04/10-13:17</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -4371,7 +4371,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>03/10-22:10</t>
+          <t>04/10-13:19</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -4381,7 +4381,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>03/10-22:12</t>
+          <t>04/10-13:20</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -4391,7 +4391,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>03/10-22:14</t>
+          <t>04/10-13:22</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -4401,7 +4401,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>03/10-22:17</t>
+          <t>04/10-13:23</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -4411,7 +4411,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>03/10-22:18</t>
+          <t>04/10-13:24</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -4421,7 +4421,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>03/10-22:20</t>
+          <t>04/10-13:26</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -4431,7 +4431,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>03/10-22:22</t>
+          <t>04/10-13:27</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -4441,7 +4441,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>03/10-22:24</t>
+          <t>04/10-13:29</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -4451,7 +4451,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>03/10-22:25</t>
+          <t>04/10-13:30</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -4461,7 +4461,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>03/10-22:27</t>
+          <t>04/10-13:32</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -4471,7 +4471,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>03/10-22:28</t>
+          <t>04/10-13:33</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -4481,7 +4481,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>03/10-22:30</t>
+          <t>04/10-13:35</t>
         </is>
       </c>
       <c r="B30" t="n">

</xml_diff>